<commit_message>
Adds Data Creation and Weather Distribution Tables
</commit_message>
<xml_diff>
--- a/design_documents/Scope_Model.xlsx
+++ b/design_documents/Scope_Model.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="27510"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/imac27/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/luciaeve/Documents/EMSE/KAISERSLAUTERN/THESIS/code/tsr_uncertainy_framework/design_documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52271D3E-599C-9C4A-AD75-ED648E728C7D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="460" windowWidth="27680" windowHeight="17040"/>
+    <workbookView xWindow="17020" yWindow="460" windowWidth="27680" windowHeight="17040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SCOPE_MODEL_DATA" sheetId="4" r:id="rId1"/>
@@ -17,16 +18,16 @@
     <sheet name="SCOPE_COMPLIANCY" sheetId="3" r:id="rId3"/>
     <sheet name="MODELS" sheetId="2" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="150001"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
-    </ext>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
 </workbook>
@@ -83,9 +84,6 @@
     <t xml:space="preserve">evaluate situation </t>
   </si>
   <si>
-    <t>image</t>
-  </si>
-  <si>
     <t xml:space="preserve">Validate context factors to specific target application scope </t>
   </si>
   <si>
@@ -185,9 +183,6 @@
     <t>temperature from current online weather forecast</t>
   </si>
   <si>
-    <t>current weather forecast</t>
-  </si>
-  <si>
     <t>RAIN_FORECAST</t>
   </si>
   <si>
@@ -312,12 +307,18 @@
   </si>
   <si>
     <t>verify_driving_direction()</t>
+  </si>
+  <si>
+    <t>environmental</t>
+  </si>
+  <si>
+    <t>imagebasedFactors</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -409,11 +410,11 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -735,11 +736,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -756,409 +757,409 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B1" s="4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E1" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="G1" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="I1" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="G1" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="I1" s="4" t="s">
+    </row>
+    <row r="2" spans="1:9" ht="68" x14ac:dyDescent="0.2">
+      <c r="A2" s="6" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" ht="64" x14ac:dyDescent="0.2">
-      <c r="A2" s="5" t="s">
+      <c r="B2" s="2" t="s">
         <v>22</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>23</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="H2" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="I2" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="H2" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="I2" s="2" t="s">
+    </row>
+    <row r="3" spans="1:9" ht="238" x14ac:dyDescent="0.2">
+      <c r="A3" s="6"/>
+      <c r="B3" s="2" t="s">
         <v>26</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" ht="224" x14ac:dyDescent="0.2">
-      <c r="A3" s="5"/>
-      <c r="B3" s="2" t="s">
-        <v>27</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D3" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="51" x14ac:dyDescent="0.2">
+      <c r="A4" s="6"/>
+      <c r="B4" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="51" x14ac:dyDescent="0.2">
+      <c r="A5" s="6"/>
+      <c r="B5" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="E3" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="48" x14ac:dyDescent="0.2">
-      <c r="A4" s="5"/>
-      <c r="B4" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="C4" s="2" t="s">
+      <c r="D5" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+      <c r="A6" s="6"/>
+      <c r="B6" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="D4" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="H4" s="2" t="s">
+      <c r="D6" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="I4" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="48" x14ac:dyDescent="0.2">
-      <c r="A5" s="5"/>
-      <c r="B5" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C5" s="2" t="s">
+      <c r="E6" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="85" x14ac:dyDescent="0.2">
+      <c r="A7" s="5"/>
+      <c r="B7" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D7" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="E5" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="I5" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" ht="32" x14ac:dyDescent="0.2">
-      <c r="A6" s="5"/>
-      <c r="B6" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="I6" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="80" x14ac:dyDescent="0.2">
-      <c r="A7" s="6"/>
-      <c r="B7" s="2" t="s">
+      <c r="E7" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C7" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="E7" s="2" t="s">
+      <c r="F7" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G7" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="F7" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="G7" s="2" t="s">
+      <c r="H7" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="64" x14ac:dyDescent="0.2">
+      <c r="A8" s="5"/>
+      <c r="B8" s="2" t="s">
         <v>42</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="I7" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="64" x14ac:dyDescent="0.2">
-      <c r="A8" s="6"/>
-      <c r="B8" s="2" t="s">
-        <v>43</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E8" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G8" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="F8" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="G8" s="2" t="s">
+      <c r="H8" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="102" x14ac:dyDescent="0.2">
+      <c r="A9" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>45</v>
-      </c>
-      <c r="H8" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="I8" s="2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" ht="96" x14ac:dyDescent="0.2">
-      <c r="A9" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>46</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>4</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" ht="128" x14ac:dyDescent="0.2">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="136" x14ac:dyDescent="0.2">
       <c r="A10" s="7"/>
       <c r="B10" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>4</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" ht="112" x14ac:dyDescent="0.2">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="119" x14ac:dyDescent="0.2">
       <c r="A11" s="7"/>
       <c r="B11" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>4</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" ht="112" x14ac:dyDescent="0.2">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="119" x14ac:dyDescent="0.2">
       <c r="A12" s="7"/>
       <c r="B12" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>4</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" ht="96" x14ac:dyDescent="0.2">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="102" x14ac:dyDescent="0.2">
       <c r="A13" s="7"/>
       <c r="B13" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>4</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" ht="96" x14ac:dyDescent="0.2">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="102" x14ac:dyDescent="0.2">
       <c r="A14" s="7"/>
       <c r="B14" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>4</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" ht="112" x14ac:dyDescent="0.2">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="119" x14ac:dyDescent="0.2">
       <c r="A15" s="7"/>
       <c r="B15" s="2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>4</v>
       </c>
       <c r="E15" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="I15" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+      <c r="A16" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="B16" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="F15" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="G15" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="I15" s="2" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" ht="32" x14ac:dyDescent="0.2">
-      <c r="A16" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>66</v>
-      </c>
       <c r="C16" s="2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A17" s="8"/>
       <c r="B17" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>5</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A18" s="8"/>
       <c r="B18" s="2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
   </sheetData>
@@ -1172,7 +1173,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1186,7 +1187,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1234,7 +1235,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1253,7 +1254,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -1266,12 +1267,12 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B3" r:id="rId1" location="G16V7ohE4z0hJQVvoX55ujsbxY6FfnvjIB"/>
+    <hyperlink ref="B3" r:id="rId1" location="G16V7ohE4z0hJQVvoX55ujsbxY6FfnvjIB" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Adds Scope Compliancy Framework
</commit_message>
<xml_diff>
--- a/design_documents/Scope_Model.xlsx
+++ b/design_documents/Scope_Model.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/luciaeve/Documents/EMSE/KAISERSLAUTERN/THESIS/code/tsr_uncertainy_framework/design_documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52271D3E-599C-9C4A-AD75-ED648E728C7D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A59B87BA-0A13-7D49-AF01-9D80B1669C3E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17020" yWindow="460" windowWidth="27680" windowHeight="17040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1720" yWindow="460" windowWidth="27680" windowHeight="17040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SCOPE_MODEL_DATA" sheetId="4" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="97">
   <si>
     <t xml:space="preserve">Scope Model </t>
   </si>
@@ -313,6 +313,24 @@
   </si>
   <si>
     <t>imagebasedFactors</t>
+  </si>
+  <si>
+    <t>generation method</t>
+  </si>
+  <si>
+    <t>randomly [within range]</t>
+  </si>
+  <si>
+    <t>randomly within range</t>
+  </si>
+  <si>
+    <t>https://elevation-api.io/api/elevation?points=</t>
+  </si>
+  <si>
+    <t>randomly generated within range</t>
+  </si>
+  <si>
+    <t>https://opendata.dwd.de/climate_environment/CDC/observations_germany/climate/monthly/more_precip/historical/</t>
   </si>
 </sst>
 </file>
@@ -400,7 +418,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -421,6 +439,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -737,10 +758,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I18"/>
+  <dimension ref="A1:J18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -755,7 +776,7 @@
     <col min="10" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" ht="32" x14ac:dyDescent="0.2">
       <c r="B1" s="4" t="s">
         <v>67</v>
       </c>
@@ -780,8 +801,11 @@
       <c r="I1" s="4" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" ht="68" x14ac:dyDescent="0.2">
+      <c r="J1" s="4" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="68" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
         <v>21</v>
       </c>
@@ -806,8 +830,11 @@
       <c r="I2" s="2" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" ht="238" x14ac:dyDescent="0.2">
+      <c r="J2" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="238" x14ac:dyDescent="0.2">
       <c r="A3" s="6"/>
       <c r="B3" s="2" t="s">
         <v>26</v>
@@ -833,8 +860,11 @@
       <c r="I3" s="2" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" ht="51" x14ac:dyDescent="0.2">
+      <c r="J3" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="85" x14ac:dyDescent="0.2">
       <c r="A4" s="6"/>
       <c r="B4" s="2" t="s">
         <v>29</v>
@@ -860,8 +890,11 @@
       <c r="I4" s="2" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" ht="51" x14ac:dyDescent="0.2">
+      <c r="J4" s="9" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="51" x14ac:dyDescent="0.2">
       <c r="A5" s="6"/>
       <c r="B5" s="2" t="s">
         <v>32</v>
@@ -884,8 +917,11 @@
       <c r="I5" s="2" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+      <c r="J5" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="68" x14ac:dyDescent="0.2">
       <c r="A6" s="6"/>
       <c r="B6" s="2" t="s">
         <v>36</v>
@@ -911,8 +947,11 @@
       <c r="I6" s="2" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" ht="85" x14ac:dyDescent="0.2">
+      <c r="J6" s="2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="85" x14ac:dyDescent="0.2">
       <c r="A7" s="5"/>
       <c r="B7" s="2" t="s">
         <v>39</v>
@@ -939,7 +978,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="64" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" ht="187" x14ac:dyDescent="0.2">
       <c r="A8" s="5"/>
       <c r="B8" s="2" t="s">
         <v>42</v>
@@ -965,8 +1004,11 @@
       <c r="I8" s="2" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" ht="102" x14ac:dyDescent="0.2">
+      <c r="J8" s="9" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="102" x14ac:dyDescent="0.2">
       <c r="A9" s="7" t="s">
         <v>89</v>
       </c>
@@ -989,7 +1031,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="136" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" ht="136" x14ac:dyDescent="0.2">
       <c r="A10" s="7"/>
       <c r="B10" s="2" t="s">
         <v>47</v>
@@ -1010,7 +1052,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="119" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" ht="119" x14ac:dyDescent="0.2">
       <c r="A11" s="7"/>
       <c r="B11" s="2" t="s">
         <v>50</v>
@@ -1031,7 +1073,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="119" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" ht="119" x14ac:dyDescent="0.2">
       <c r="A12" s="7"/>
       <c r="B12" s="2" t="s">
         <v>53</v>
@@ -1052,7 +1094,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="102" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" ht="102" x14ac:dyDescent="0.2">
       <c r="A13" s="7"/>
       <c r="B13" s="2" t="s">
         <v>56</v>
@@ -1073,7 +1115,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="102" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10" ht="102" x14ac:dyDescent="0.2">
       <c r="A14" s="7"/>
       <c r="B14" s="2" t="s">
         <v>59</v>
@@ -1094,7 +1136,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="119" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10" ht="119" x14ac:dyDescent="0.2">
       <c r="A15" s="7"/>
       <c r="B15" s="2" t="s">
         <v>61</v>
@@ -1115,7 +1157,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A16" s="8" t="s">
         <v>90</v>
       </c>
@@ -1168,6 +1210,10 @@
     <mergeCell ref="A9:A15"/>
     <mergeCell ref="A16:A18"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="J4" r:id="rId1" xr:uid="{9DAF59C8-EABD-FA46-9B2F-B6EC4446C8D7}"/>
+    <hyperlink ref="J8" r:id="rId2" xr:uid="{46E905E8-FDEB-8C47-A3A2-DD0131B641B9}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Adds data set additions
</commit_message>
<xml_diff>
--- a/design_documents/Scope_Model.xlsx
+++ b/design_documents/Scope_Model.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10412"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/luciaeve/Documents/EMSE/KAISERSLAUTERN/THESIS/code/tsr_uncertainy_framework/design_documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9853D0FB-E4DC-5C4F-91BD-720FE31B9142}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A269A28B-6A25-FE4F-B491-030D40812CD1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="27680" windowHeight="17040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,7 +18,7 @@
     <sheet name="SCOPE_COMPLIANCY" sheetId="3" r:id="rId3"/>
     <sheet name="MODELS" sheetId="2" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="150001"/>
+  <calcPr calcId="150001" calcCompleted="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="102">
   <si>
     <t xml:space="preserve">Scope Model </t>
   </si>
@@ -327,13 +327,25 @@
     <t>https://elevation-api.io/api/elevation?points=</t>
   </si>
   <si>
-    <t>randomly generated within range</t>
-  </si>
-  <si>
     <t>https://opendata.dwd.de/climate_environment/CDC/observations_germany/climate/monthly/more_precip/historical/</t>
   </si>
   <si>
     <t>weather_data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">based on open_data returned type </t>
+  </si>
+  <si>
+    <t>open_data</t>
+  </si>
+  <si>
+    <t>from GTSBR {labelled}</t>
+  </si>
+  <si>
+    <t>right</t>
+  </si>
+  <si>
+    <t>10% left</t>
   </si>
 </sst>
 </file>
@@ -761,10 +773,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J18"/>
+  <dimension ref="A1:J19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -868,7 +880,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="85" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" ht="51" x14ac:dyDescent="0.2">
       <c r="A4" s="7"/>
       <c r="B4" s="2" t="s">
         <v>29</v>
@@ -925,7 +937,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="68" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A6" s="7"/>
       <c r="B6" s="2" t="s">
         <v>36</v>
@@ -952,7 +964,7 @@
         <v>38</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="85" x14ac:dyDescent="0.2">
@@ -982,7 +994,7 @@
         <v>41</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="187" x14ac:dyDescent="0.2">
@@ -1012,7 +1024,7 @@
         <v>44</v>
       </c>
       <c r="J8" s="6" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="102" x14ac:dyDescent="0.2">
@@ -1180,8 +1192,11 @@
       <c r="F16" s="2" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="J16" s="2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A17" s="9"/>
       <c r="B17" s="2" t="s">
         <v>65</v>
@@ -1195,8 +1210,11 @@
       <c r="F17" s="2" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="J17" s="2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A18" s="9"/>
       <c r="B18" s="2" t="s">
         <v>66</v>
@@ -1209,6 +1227,14 @@
       </c>
       <c r="F18" s="2" t="s">
         <v>76</v>
+      </c>
+      <c r="J18" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="J19" s="2" t="s">
+        <v>101</v>
       </c>
     </row>
   </sheetData>

</xml_diff>